<commit_message>
Aesthetics on draft graphs
</commit_message>
<xml_diff>
--- a/docs/Graphs.xlsx
+++ b/docs/Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmoran/Desktop/thesis/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9ED553-4667-6944-93AC-CB8243B80D17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D1E88A-AA98-9C44-96BC-9C93AC25E3CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="900" windowWidth="33820" windowHeight="18940" activeTab="1" xr2:uid="{B2B47576-883A-3F4F-8CBA-62FB005EF20E}"/>
+    <workbookView xWindow="2240" yWindow="460" windowWidth="33820" windowHeight="18940" activeTab="2" xr2:uid="{B2B47576-883A-3F4F-8CBA-62FB005EF20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs Data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Graphs!$A$1:$M$36</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="33">
   <si>
     <t>trend</t>
   </si>
@@ -92,9 +92,6 @@
     <t>strict_ar1</t>
   </si>
   <si>
-    <t>naive</t>
-  </si>
-  <si>
     <t>ar1_diff</t>
   </si>
   <si>
@@ -135,6 +132,12 @@
   </si>
   <si>
     <t>Inflation</t>
+  </si>
+  <si>
+    <t>Naïve forecast</t>
+  </si>
+  <si>
+    <t>Non-sample based forest model</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -1811,7 +1814,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -3424,7 +3427,7 @@
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
-        <c:majorUnit val="12"/>
+        <c:majorUnit val="36"/>
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
@@ -3532,9 +3535,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13642825896762906"/>
-          <c:y val="7.6423519976669588E-2"/>
-          <c:w val="0.863571741032371"/>
+          <c:x val="0.10090288346394764"/>
+          <c:y val="3.2126587624822761E-2"/>
+          <c:w val="0.82055314118557954"/>
           <c:h val="0.89814814814814814"/>
         </c:manualLayout>
       </c:layout>
@@ -3556,7 +3559,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -5123,7 +5126,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -6736,7 +6739,7 @@
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
-        <c:majorUnit val="12"/>
+        <c:majorUnit val="36"/>
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
@@ -6745,7 +6748,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="r"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -6792,7 +6795,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1642124656"/>
-        <c:crosses val="max"/>
+        <c:crossesAt val="36161"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
@@ -6868,7 +6871,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -8435,7 +8438,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -10048,7 +10051,7 @@
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
-        <c:majorUnit val="12"/>
+        <c:majorUnit val="36"/>
         <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
@@ -10170,17 +10173,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Graphs Data'!$G$1</c:f>
+              <c:f>'Graphs Data'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>naive</c:v>
+                  <c:v>Non-sample based forest model</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
@@ -10959,768 +10962,768 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graphs Data'!$G$2:$G$254</c:f>
+              <c:f>'Graphs Data'!$C$2:$C$254</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="253"/>
                 <c:pt idx="0">
-                  <c:v>1.8264845260347301E-3</c:v>
+                  <c:v>1.92255103428362E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.82315456151461E-3</c:v>
+                  <c:v>2.1183229329529E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1.3494218117949899E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.0698029177697098E-4</c:v>
+                  <c:v>1.5065414614180801E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6525797210275099E-3</c:v>
+                  <c:v>3.7031576159388098E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0259116014460502E-4</c:v>
+                  <c:v>1.9987153008460701E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.4671034390494901E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.2080014002046102E-3</c:v>
+                  <c:v>1.9405454256298099E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.3966458446000902E-3</c:v>
+                  <c:v>1.8267325040027399E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.1803584317578997E-3</c:v>
+                  <c:v>2.1332205036672602E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.78624638146374E-3</c:v>
+                  <c:v>1.8952533543776099E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.7830613936560299E-3</c:v>
+                  <c:v>2.21615561538191E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.3724803536309099E-3</c:v>
+                  <c:v>2.0041561172728299E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9577069772326299E-3</c:v>
+                  <c:v>2.1555496901908399E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.1261479111724996E-3</c:v>
+                  <c:v>2.4144558025134401E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.8651194523981999E-3</c:v>
+                  <c:v>3.2751833249138099E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-5.8496638111460398E-4</c:v>
+                  <c:v>2.2749056956076598E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.7538735860957999E-3</c:v>
+                  <c:v>2.5410854775011001E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.8241282859885501E-3</c:v>
+                  <c:v>2.0255485619187501E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8993931590024502E-3</c:v>
+                  <c:v>2.7243858155884299E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>3.1010903580574898E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.19781707361755E-3</c:v>
+                  <c:v>2.2330602084074101E-3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.7266191339873099E-3</c:v>
+                  <c:v>2.9567718641365401E-3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.7236430581650799E-3</c:v>
+                  <c:v>2.40738501342515E-3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2935789870990298E-3</c:v>
+                  <c:v>1.9993982738900299E-3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.7110377955149599E-3</c:v>
+                  <c:v>2.1669937705825E-3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.27531383713497E-3</c:v>
+                  <c:v>3.2044901478126601E-3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.6802046400861205E-4</c:v>
+                  <c:v>3.2507988297340901E-3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.70212807053094E-3</c:v>
+                  <c:v>1.8996088068797201E-3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.08906950747168E-3</c:v>
+                  <c:v>2.25922803727575E-3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.2535220804433798E-3</c:v>
+                  <c:v>2.6324359755210401E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1.68966528512726E-3</c:v>
+                  <c:v>3.1407193311705798E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>1.84668268756332E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.9381204201376398E-3</c:v>
+                  <c:v>2.7428491765689E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-2.81135973754676E-3</c:v>
+                  <c:v>1.16199904169664E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-5.6322164259903196E-4</c:v>
+                  <c:v>1.7956133172000201E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-5.6353903999184496E-4</c:v>
+                  <c:v>1.12399765187096E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.68966528512726E-3</c:v>
+                  <c:v>2.10682812070522E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.68681513147906E-3</c:v>
+                  <c:v>2.10349075455244E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.8050509276083E-3</c:v>
+                  <c:v>2.5930477513647098E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.4717793913937598E-3</c:v>
+                  <c:v>3.1913206065499302E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.1148273172460999E-3</c:v>
+                  <c:v>1.8308885680410501E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.5694793976623902E-4</c:v>
+                  <c:v>1.4230930939094701E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.2246950221109802E-3</c:v>
+                  <c:v>2.2249529482537898E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.7739268827256E-3</c:v>
+                  <c:v>2.0657241289585098E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.6606701851404899E-3</c:v>
+                  <c:v>2.0019728453084E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.20994565080268E-3</c:v>
+                  <c:v>2.3737861575979999E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.65426009602587E-3</c:v>
+                  <c:v>2.0702748613544699E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.65152803847324E-3</c:v>
+                  <c:v>2.1533457535448598E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.39078641749013E-3</c:v>
+                  <c:v>2.3233607639760799E-3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.4615100255217498E-3</c:v>
+                  <c:v>4.0905742903639599E-3</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.63265342388552E-3</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>-3.8136793702454601E-3</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>-1.63889684321017E-3</c:v>
+                  <c:v>1.6427151438027699E-3</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="0.00E+00">
+                  <c:v>5.3863264770440903E-4</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="0.00E+00">
+                  <c:v>6.8892956261034797E-4</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.0928962836445101E-3</c:v>
+                  <c:v>1.8779785507587101E-3</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>3.2715405406156298E-3</c:v>
+                  <c:v>2.83046289150884E-3</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.3454712595014698E-3</c:v>
+                  <c:v>3.4242841076193601E-3</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>3.2467560988704799E-3</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>-1.0810811863732901E-3</c:v>
+                  <c:v>2.8393506529751302E-3</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="0.00E+00">
+                  <c:v>7.6152648668204005E-4</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.4068668524553899E-4</c:v>
+                  <c:v>1.95840990951351E-3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.69905696916517E-3</c:v>
+                  <c:v>2.60731771124774E-3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.3033955600533203E-3</c:v>
+                  <c:v>2.8390623778307999E-3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.1447729401336E-3</c:v>
+                  <c:v>1.8358017829416401E-3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.1401827323677099E-3</c:v>
+                  <c:v>2.25758415950394E-3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.60213652427732E-3</c:v>
+                  <c:v>2.1593190294952901E-3</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.2598573469581104E-3</c:v>
+                  <c:v>2.38270004522128E-3</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.7125473561845398E-3</c:v>
+                  <c:v>1.6180281098877301E-3</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.0582011569475499E-3</c:v>
+                  <c:v>1.2503057675415799E-3</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.2868095336577902E-4</c:v>
+                  <c:v>1.8529239940060201E-3</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>3.16622955805013E-3</c:v>
+                  <c:v>2.2551330883639198E-3</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.2548728383587902E-3</c:v>
+                  <c:v>3.3007724196348E-3</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.7058910374122602E-3</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0</c:v>
+                  <c:v>2.86122321766847E-3</c:v>
+                </c:pt>
+                <c:pt idx="72" formatCode="0.00E+00">
+                  <c:v>5.5506545150580105E-4</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-5.2178451483886302E-4</c:v>
+                  <c:v>1.59716545123992E-3</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.1666726948461604E-3</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>3.6316512028626798E-3</c:v>
+                  <c:v>3.8776144124875399E-3</c:v>
+                </c:pt>
+                <c:pt idx="75" formatCode="0.00E+00">
+                  <c:v>7.8706136667281096E-4</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>3.10238097848181E-3</c:v>
+                  <c:v>1.1510023513875401E-3</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-5.1639557047344898E-4</c:v>
+                  <c:v>1.81411430274227E-3</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.1639557047344898E-4</c:v>
+                  <c:v>2.2389601104326E-3</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6.1760361005642698E-3</c:v>
+                  <c:v>4.6588967884315701E-3</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>6.1381266887856603E-3</c:v>
+                  <c:v>3.5940584207535598E-3</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.3674561020173399E-2</c:v>
+                  <c:v>8.3933100913488393E-3</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.5079168476770401E-3</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>-5.0352573656455802E-3</c:v>
+                  <c:v>2.09741673436081E-3</c:v>
+                </c:pt>
+                <c:pt idx="83" formatCode="0.00E+00">
+                  <c:v>3.3895773333270302E-4</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0</c:v>
+                  <c:v>1.6772970706242301E-3</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>6.0392735142436003E-3</c:v>
+                  <c:v>3.2788189770285199E-3</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>5.0163030898886496E-4</c:v>
+                  <c:v>1.8513180542799801E-3</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.5033828940316199E-3</c:v>
+                  <c:v>2.10201654416275E-3</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.9950153805227203E-3</c:v>
+                  <c:v>2.9915206036434799E-3</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2.9850768434540602E-3</c:v>
+                  <c:v>2.5453277909202798E-3</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.48077527376278E-3</c:v>
+                  <c:v>2.3622049419295501E-3</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>5.4361389122599101E-3</c:v>
+                  <c:v>3.1091096294162501E-3</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.4258739568556697E-3</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>-4.91884907159612E-3</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>-4.4477463982364202E-3</c:v>
+                  <c:v>2.8451595831425099E-3</c:v>
+                </c:pt>
+                <c:pt idx="93" formatCode="0.00E+00">
+                  <c:v>5.49921048437781E-4</c:v>
+                </c:pt>
+                <c:pt idx="94" formatCode="0.00E+00">
+                  <c:v>4.9749445612583796E-4</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>4.9517208241312005E-4</c:v>
+                  <c:v>1.80071201274801E-3</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>5.4307711851340201E-3</c:v>
+                  <c:v>3.0978926767696899E-3</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.65790605623251E-3</c:v>
+                  <c:v>2.3516658488723298E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3.8708491335395201E-3</c:v>
+                  <c:v>2.76829474821589E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>5.1866474931996399E-3</c:v>
+                  <c:v>3.0379228464997E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.9961694819986601E-3</c:v>
+                  <c:v>2.4865385635404699E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>4.12447665692373E-3</c:v>
+                  <c:v>2.76926770530529E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.3140721794590001E-3</c:v>
+                  <c:v>2.3039671841504402E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.779012466681E-3</c:v>
+                  <c:v>2.1667309540258201E-3</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>3.0823320011830202E-4</c:v>
+                  <c:v>1.7734064325732499E-3</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>4.2286002454385904E-3</c:v>
+                  <c:v>2.7900476174955598E-3</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>3.0784944010990899E-3</c:v>
+                  <c:v>2.5012809830688501E-3</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>7.8281640828734601E-3</c:v>
+                  <c:v>3.7257062373534499E-3</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.8938234029487501E-3</c:v>
+                  <c:v>2.3753421964255502E-3</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>3.4417753671736099E-3</c:v>
+                  <c:v>2.60684675912386E-3</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.4149086374540799E-3</c:v>
+                  <c:v>2.3462131487541702E-3</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>3.5716418927451699E-3</c:v>
+                  <c:v>2.6400874314112298E-3</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.3117069655080899E-3</c:v>
+                  <c:v>2.3110907613868199E-3</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>5.9000520681236103E-3</c:v>
+                  <c:v>3.2316710491423701E-3</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.0423718797166101E-2</c:v>
+                  <c:v>6.5036708400606404E-3</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>7.1160653935047301E-3</c:v>
+                  <c:v>4.8507093210361897E-3</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>-1.4895846082953999E-3</c:v>
+                  <c:v>1.3601044616548101E-3</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>8.5472629967320302E-4</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>-8.6356163995580104E-3</c:v>
+                  <c:v>1.9598613606679502E-3</c:v>
+                </c:pt>
+                <c:pt idx="118" formatCode="0.00E+00">
+                  <c:v>-6.3236384030488204E-4</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>-1.7864094092818299E-2</c:v>
+                  <c:v>-8.1647430478651601E-3</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>-8.26760505408153E-3</c:v>
+                  <c:v>-3.07664503700826E-3</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.5275743322667999E-3</c:v>
+                  <c:v>2.5143633288361401E-3</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>3.6360422314452002E-3</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>-9.8777054127285901E-4</c:v>
+                  <c:v>3.0757964174220002E-3</c:v>
+                </c:pt>
+                <c:pt idx="123" formatCode="0.00E+00">
+                  <c:v>7.3335826296611604E-4</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>1.0065757521973101E-3</c:v>
+                  <c:v>1.7418245858593199E-3</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>1.4704123326474399E-3</c:v>
+                  <c:v>1.9749494482484498E-3</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>8.26535985544119E-3</c:v>
+                  <c:v>5.4097165506657701E-3</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>-2.9800985515571199E-4</c:v>
+                  <c:v>1.1068515016718901E-3</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>3.34285979087934E-3</c:v>
+                  <c:v>2.92869239155925E-3</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>1.92902546683626E-3</c:v>
+                  <c:v>2.2221893306454701E-3</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>2.9974349985852902E-3</c:v>
+                  <c:v>2.7552990680610998E-3</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>3.3429965449309801E-3</c:v>
+                  <c:v>2.9277320238848899E-3</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>5.2004115479764601E-4</c:v>
+                  <c:v>1.51742270389495E-3</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>6.48521875846519E-4</c:v>
+                  <c:v>1.6326433210543201E-3</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>-9.52229876745037E-4</c:v>
+                  <c:v>1.0891528239428099E-3</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>3.3131324589685801E-4</c:v>
+                  <c:v>1.51120928991215E-3</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>2.30014077875929E-4</c:v>
+                  <c:v>1.4709222019921699E-3</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>-5.1990716457517305E-4</c:v>
+                  <c:v>1.10652153078533E-3</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>-4.1888287772806599E-4</c:v>
+                  <c:v>1.2329659834318201E-3</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>1.8675086613582101E-3</c:v>
+                  <c:v>2.0059026891549301E-3</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>1.4602967272390199E-3</c:v>
+                  <c:v>1.94232931665447E-3</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>1.6139463106572499E-3</c:v>
+                  <c:v>1.9171056840002699E-3</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>3.4757987017952599E-3</c:v>
+                  <c:v>2.8208422454814698E-3</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>2.5306368592339398E-3</c:v>
+                  <c:v>2.2290753063862099E-3</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>4.0085314388491602E-3</c:v>
+                  <c:v>3.2418604777470902E-3</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>3.2377948808060002E-3</c:v>
+                  <c:v>2.8551930032151098E-3</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>3.2093192514253098E-3</c:v>
+                  <c:v>2.8408540954755301E-3</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>5.1602113856565896E-3</c:v>
+                  <c:v>3.8206094505416899E-3</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>4.6831160490556903E-3</c:v>
+                  <c:v>3.58215406727242E-3</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>3.1766637911196899E-3</c:v>
+                  <c:v>2.8264986567945499E-3</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>0</c:v>
+                  <c:v>1.38374173741026E-3</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>2.6166105186638E-3</c:v>
+                  <c:v>2.2697713268882399E-3</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>3.1494972889110099E-3</c:v>
+                  <c:v>2.8109057259106699E-3</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>2.1691934558836202E-3</c:v>
+                  <c:v>2.11979997655431E-3</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>6.7497967697516302E-4</c:v>
+                  <c:v>1.61274658858379E-3</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>1.8461448804947299E-3</c:v>
+                  <c:v>2.0070742401178099E-3</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>2.3768024196879601E-4</c:v>
+                  <c:v>1.4600424813513901E-3</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>2.72049215726167E-3</c:v>
+                  <c:v>2.2991285252377202E-3</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>2.1351650368677299E-3</c:v>
+                  <c:v>2.1016602575584598E-3</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>2.0912821313983101E-3</c:v>
+                  <c:v>2.0597565908448698E-3</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>1.65941076607456E-3</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>-2.0703217702822099E-3</c:v>
+                  <c:v>1.93971255661042E-3</c:v>
+                </c:pt>
+                <c:pt idx="161" formatCode="0.00E+00">
+                  <c:v>6.71146901638233E-4</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>-8.26704797574074E-4</c:v>
+                  <c:v>1.07865931059025E-3</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>2.8876823050083501E-4</c:v>
+                  <c:v>1.4522805475250501E-3</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>5.7927177431231804E-3</c:v>
+                  <c:v>3.3236151577223198E-3</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>4.7599198634582498E-3</c:v>
+                  <c:v>2.9806386969604601E-3</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>2.69316475440018E-3</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>-1.6807561740774799E-3</c:v>
+                  <c:v>2.2815647570007501E-3</c:v>
+                </c:pt>
+                <c:pt idx="167" formatCode="0.00E+00">
+                  <c:v>7.9830746884685798E-4</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>-1.21088935646441E-4</c:v>
+                  <c:v>1.31785257879655E-3</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>1.9788297664797799E-3</c:v>
+                  <c:v>2.0290309566428199E-3</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>5.4152378489549201E-3</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>-2.81587997395238E-3</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>-2.09016213434055E-3</c:v>
+                  <c:v>3.1947947884163599E-3</c:v>
+                </c:pt>
+                <c:pt idx="171" formatCode="0.00E+00">
+                  <c:v>4.4304555441666702E-4</c:v>
+                </c:pt>
+                <c:pt idx="172" formatCode="0.00E+00">
+                  <c:v>6.5741505022251599E-4</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>4.1406975078839303E-4</c:v>
+                  <c:v>1.49375115417713E-3</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>2.3775795219549401E-3</c:v>
+                  <c:v>2.15261827596491E-3</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>1.9555389871959202E-3</c:v>
+                  <c:v>2.0107161232714998E-3</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>2.3844456313710802E-3</c:v>
+                  <c:v>2.1544287185401201E-3</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>3.7687366613159401E-4</c:v>
+                  <c:v>1.4792704457527201E-3</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>5.3508786348999105E-4</c:v>
+                  <c:v>1.5280024685912E-3</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>1.84279044557734E-3</c:v>
+                  <c:v>1.9660382135877198E-3</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>2.6406794933659899E-3</c:v>
+                  <c:v>2.2340437894177302E-3</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>2.42124171757485E-3</c:v>
+                  <c:v>2.22453074080463E-3</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>1.10017320770073E-3</c:v>
+                  <c:v>1.8292326979122101E-3</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>2.03997314024917E-3</c:v>
+                  <c:v>2.03068229436948E-3</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>1.8624501675628101E-3</c:v>
+                  <c:v>1.9704789861216599E-3</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>1.9011974817404499E-3</c:v>
+                  <c:v>1.9827963500921599E-3</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>1.3202602787965E-3</c:v>
+                  <c:v>1.7864356542510501E-3</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>1.12485240275095E-3</c:v>
+                  <c:v>1.7186921025740801E-3</c:v>
                 </c:pt>
                 <c:pt idx="188">
-                  <c:v>-1.6001414896038601E-4</c:v>
-                </c:pt>
-                <c:pt idx="189" formatCode="0.00E+00">
-                  <c:v>7.1588442287051594E-5</c:v>
+                  <c:v>1.28164415777827E-3</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>1.35351441462055E-3</c:v>
                 </c:pt>
                 <c:pt idx="190">
-                  <c:v>-1.97933490782454E-4</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>-1.8844345845421299E-3</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>-3.0893766581243701E-3</c:v>
+                  <c:v>1.2555264705353499E-3</c:v>
+                </c:pt>
+                <c:pt idx="191" formatCode="0.00E+00">
+                  <c:v>6.6723533168117403E-4</c:v>
+                </c:pt>
+                <c:pt idx="192" formatCode="0.00E+00">
+                  <c:v>-3.9146010019876101E-4</c:v>
                 </c:pt>
                 <c:pt idx="193">
-                  <c:v>-6.3906934924871104E-3</c:v>
+                  <c:v>-2.1067854135744602E-3</c:v>
                 </c:pt>
                 <c:pt idx="194">
-                  <c:v>2.5314368884981099E-3</c:v>
+                  <c:v>2.4429339928186099E-3</c:v>
                 </c:pt>
                 <c:pt idx="195">
-                  <c:v>2.69032959658144E-3</c:v>
+                  <c:v>2.5225692813080599E-3</c:v>
                 </c:pt>
                 <c:pt idx="196">
-                  <c:v>1.04193589238211E-3</c:v>
+                  <c:v>1.6349660059255199E-3</c:v>
                 </c:pt>
                 <c:pt idx="197">
-                  <c:v>3.29231970405353E-3</c:v>
+                  <c:v>2.41256970595621E-3</c:v>
                 </c:pt>
                 <c:pt idx="198">
-                  <c:v>2.7640971717151101E-3</c:v>
+                  <c:v>2.2313934139321398E-3</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>1.5850629039944101E-3</c:v>
-                </c:pt>
-                <c:pt idx="200" formatCode="0.00E+00">
-                  <c:v>-4.20108934306995E-6</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>-2.2501171352722299E-3</c:v>
+                  <c:v>1.8245176254582101E-3</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1.27296719410299E-3</c:v>
+                </c:pt>
+                <c:pt idx="201" formatCode="0.00E+00">
+                  <c:v>4.8036344665795502E-4</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>9.889928020463401E-4</c:v>
+                  <c:v>1.52918401049795E-3</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>1.1939045033511099E-3</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>-1.0761322495165301E-3</c:v>
+                  <c:v>1.71198345017089E-3</c:v>
+                </c:pt>
+                <c:pt idx="204" formatCode="0.00E+00">
+                  <c:v>7.9346703640940995E-4</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>2.7755115950611802E-4</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>-1.31694949620442E-3</c:v>
+                  <c:v>1.3454376154352599E-3</c:v>
+                </c:pt>
+                <c:pt idx="206" formatCode="0.00E+00">
+                  <c:v>5.5295725285533495E-4</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>2.0020868762316E-3</c:v>
+                  <c:v>1.23314308885153E-3</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>3.5442809608090499E-3</c:v>
+                  <c:v>2.4655647935802301E-3</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>2.5299266016132198E-3</c:v>
+                  <c:v>2.0861586183203401E-3</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>2.9358798695158202E-3</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>-1.37426992127487E-4</c:v>
+                  <c:v>1.6403756107226299E-3</c:v>
+                </c:pt>
+                <c:pt idx="211" formatCode="0.00E+00">
+                  <c:v>9.1665672567703405E-4</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>2.01370552292701E-3</c:v>
+                  <c:v>1.75598041620089E-3</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>1.96402942325413E-3</c:v>
+                  <c:v>1.9270124961241399E-3</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>2.3741022816485798E-3</c:v>
+                  <c:v>2.0961117199498002E-3</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>1.4556464688366699E-3</c:v>
+                  <c:v>1.43575197411888E-3</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>2.9667551494805301E-3</c:v>
+                  <c:v>2.27477730567348E-3</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>4.1321608292692602E-3</c:v>
+                  <c:v>2.6814400605374399E-3</c:v>
                 </c:pt>
                 <c:pt idx="218">
-                  <c:v>1.27525671056716E-3</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>-1.25884436684309E-3</c:v>
+                  <c:v>1.69135753382575E-3</c:v>
+                </c:pt>
+                <c:pt idx="219" formatCode="0.00E+00">
+                  <c:v>8.0725835701536295E-4</c:v>
                 </c:pt>
                 <c:pt idx="220">
-                  <c:v>1.3817735229251201E-3</c:v>
+                  <c:v>1.7221207628648099E-3</c:v>
                 </c:pt>
                 <c:pt idx="221">
-                  <c:v>-5.4100135750179102E-4</c:v>
+                  <c:v>1.0213410789440399E-3</c:v>
                 </c:pt>
                 <c:pt idx="222">
-                  <c:v>1.03666228642485E-3</c:v>
+                  <c:v>1.3916825081440899E-3</c:v>
                 </c:pt>
                 <c:pt idx="223">
-                  <c:v>6.1002198380144502E-4</c:v>
+                  <c:v>1.23574868772125E-3</c:v>
                 </c:pt>
                 <c:pt idx="224">
-                  <c:v>3.9866728182635898E-3</c:v>
+                  <c:v>2.6177252971283402E-3</c:v>
                 </c:pt>
                 <c:pt idx="225">
-                  <c:v>4.6405871598045297E-3</c:v>
+                  <c:v>2.8485877178375499E-3</c:v>
                 </c:pt>
                 <c:pt idx="226">
-                  <c:v>5.0708397382859304E-4</c:v>
+                  <c:v>1.2548742802900999E-3</c:v>
                 </c:pt>
                 <c:pt idx="227">
-                  <c:v>3.0896779609497198E-3</c:v>
+                  <c:v>2.3094195175411098E-3</c:v>
                 </c:pt>
                 <c:pt idx="228">
-                  <c:v>2.0760135086410601E-3</c:v>
+                  <c:v>1.9609042096187701E-3</c:v>
                 </c:pt>
                 <c:pt idx="229">
-                  <c:v>3.9020471808726099E-3</c:v>
+                  <c:v>2.5905982949803101E-3</c:v>
                 </c:pt>
                 <c:pt idx="230">
-                  <c:v>2.64504229139462E-3</c:v>
+                  <c:v>2.15937284087841E-3</c:v>
                 </c:pt>
                 <c:pt idx="231">
-                  <c:v>-2.4855278266500098E-4</c:v>
+                  <c:v>1.1633478180158401E-3</c:v>
                 </c:pt>
                 <c:pt idx="232">
-                  <c:v>2.17874608083868E-3</c:v>
+                  <c:v>1.9965954520235001E-3</c:v>
                 </c:pt>
                 <c:pt idx="233">
-                  <c:v>2.7287435753864399E-3</c:v>
+                  <c:v>2.1856252435394799E-3</c:v>
                 </c:pt>
                 <c:pt idx="234">
-                  <c:v>2.1362419844628299E-3</c:v>
+                  <c:v>1.9827291972187799E-3</c:v>
                 </c:pt>
                 <c:pt idx="235">
-                  <c:v>1.2175277735577701E-3</c:v>
+                  <c:v>1.6669102498581101E-3</c:v>
                 </c:pt>
                 <c:pt idx="236">
-                  <c:v>1.6806159061024701E-3</c:v>
+                  <c:v>1.82475591990288E-3</c:v>
                 </c:pt>
                 <c:pt idx="237">
-                  <c:v>1.41223350708852E-3</c:v>
+                  <c:v>1.7317397347865399E-3</c:v>
                 </c:pt>
                 <c:pt idx="238">
-                  <c:v>2.0434113058724898E-3</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>-4.5504997431677902E-4</c:v>
-                </c:pt>
-                <c:pt idx="240" formatCode="0.00E+00">
-                  <c:v>-3.56213451055964E-5</c:v>
+                  <c:v>1.9477404254995001E-3</c:v>
+                </c:pt>
+                <c:pt idx="239" formatCode="0.00E+00">
+                  <c:v>8.4652452649379699E-4</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1.04344902317682E-3</c:v>
                 </c:pt>
                 <c:pt idx="241">
-                  <c:v>-4.0775688753669198E-4</c:v>
+                  <c:v>1.0387790526212701E-3</c:v>
                 </c:pt>
                 <c:pt idx="242">
-                  <c:v>2.4953990458849201E-3</c:v>
+                  <c:v>1.9164391605212901E-3</c:v>
                 </c:pt>
                 <c:pt idx="243">
-                  <c:v>3.6035648801666701E-3</c:v>
+                  <c:v>2.47539297281442E-3</c:v>
                 </c:pt>
                 <c:pt idx="244">
-                  <c:v>3.3317779201258398E-3</c:v>
+                  <c:v>2.3836814700561601E-3</c:v>
                 </c:pt>
                 <c:pt idx="245">
-                  <c:v>8.7824200426478405E-4</c:v>
+                  <c:v>1.3479503875794201E-3</c:v>
                 </c:pt>
                 <c:pt idx="246">
-                  <c:v>9.2054165683741495E-4</c:v>
+                  <c:v>1.3851790884806901E-3</c:v>
                 </c:pt>
                 <c:pt idx="247">
-                  <c:v>2.6784560744141902E-3</c:v>
+                  <c:v>2.0001303198614001E-3</c:v>
                 </c:pt>
                 <c:pt idx="248">
-                  <c:v>8.0799253392171999E-4</c:v>
+                  <c:v>1.3350153053673401E-3</c:v>
                 </c:pt>
                 <c:pt idx="249">
-                  <c:v>1.1659489668201001E-3</c:v>
+                  <c:v>1.44925462167389E-3</c:v>
                 </c:pt>
                 <c:pt idx="250">
-                  <c:v>2.47556673247473E-3</c:v>
+                  <c:v>2.0215213857713299E-3</c:v>
                 </c:pt>
                 <c:pt idx="251">
-                  <c:v>2.3104428658138301E-3</c:v>
+                  <c:v>2.0280823865784902E-3</c:v>
                 </c:pt>
                 <c:pt idx="252">
-                  <c:v>2.4018544556705401E-3</c:v>
+                  <c:v>2.0597103487419301E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11733,7 +11736,7 @@
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="13"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -11747,7 +11750,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="12700">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
@@ -13295,7 +13298,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-37C9-994B-A77E-A7C331A181FD}"/>
+              <c16:uniqueId val="{00000006-CD9C-D54E-BEF3-F607D5DE8556}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -13360,7 +13363,8 @@
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
-        <c:majorUnit val="12"/>
+        <c:majorUnit val="36"/>
+        <c:majorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
         <c:axId val="1675200800"/>
@@ -13386,7 +13390,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -14016,7 +14020,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -15243,15 +15247,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>109</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>148660</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>816428</xdr:colOff>
+      <xdr:colOff>809958</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>161360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15278,16 +15282,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>7256</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>806841</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>148849</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>823685</xdr:colOff>
+      <xdr:colOff>788975</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>159928</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15316,16 +15320,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>806550</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>157566</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>816428</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>787651</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>167592</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15354,16 +15358,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>7256</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>186872</xdr:rowOff>
+      <xdr:rowOff>157582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>823685</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>809849</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171237</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -15770,7 +15774,7 @@
   <dimension ref="A1:R254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15780,55 +15784,55 @@
         <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>21</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>23</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>24</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>26</v>
-      </c>
-      <c r="R1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
@@ -30009,8 +30013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BCF9877-9F4A-BC44-AB56-14356FEF6D7E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30025,7 +30029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD05F54-52A0-5543-BE29-AD3A645F2976}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create adjusted forecast script
</commit_message>
<xml_diff>
--- a/docs/Graphs.xlsx
+++ b/docs/Graphs.xlsx
@@ -8,16 +8,47 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexmoran/Desktop/thesis/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98D1E88A-AA98-9C44-96BC-9C93AC25E3CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{537C7416-64CF-4648-8BD4-70B594847610}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="460" windowWidth="33820" windowHeight="18940" activeTab="2" xr2:uid="{B2B47576-883A-3F4F-8CBA-62FB005EF20E}"/>
+    <workbookView xWindow="7420" yWindow="1220" windowWidth="33820" windowHeight="18940" activeTab="3" xr2:uid="{B2B47576-883A-3F4F-8CBA-62FB005EF20E}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphs Data" sheetId="1" r:id="rId1"/>
     <sheet name="Graphs" sheetId="3" r:id="rId2"/>
     <sheet name="Mentions" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$17:$C$28</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v2.18" hidden="1">Sheet1!$A$17:$A$28</definedName>
+    <definedName name="_xlchart.v2.19" hidden="1">Sheet1!$B$17:$B$28</definedName>
+    <definedName name="_xlchart.v2.20" hidden="1">Sheet1!$C$17:$C$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Graphs!$A$1:$M$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1326" uniqueCount="39">
   <si>
     <t>trend</t>
   </si>
@@ -139,12 +170,33 @@
   <si>
     <t>Non-sample based forest model</t>
   </si>
+  <si>
+    <t>real_trees</t>
+  </si>
+  <si>
+    <t>Base tree</t>
+  </si>
+  <si>
+    <t>Time series tree</t>
+  </si>
+  <si>
+    <t>% difference from base tree</t>
+  </si>
+  <si>
+    <t>Base</t>
+  </si>
+  <si>
+    <t>Time-Series</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="175" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,6 +209,13 @@
       <color theme="1"/>
       <name val="Lucida Grande"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,18 +235,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -14154,6 +14219,514 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:uLnTx/>
+                <a:uFillTx/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>Chart Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$17:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>trend</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tmin1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tmin2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tmin3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tmin4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tmin5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tmin6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tmin7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tmin8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tmin9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tmin10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tmin11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>6.4363029362207974E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.34875230699932952</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12525613191167184</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2637047703388392E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.8726389823510827E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.7560723594749684E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5623321305806049E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.8631598559126452E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.7820557551126038E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.10588703401754423</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.1406948180062379E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3334910991476747E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6DF7-434A-9D35-23966EC2FE35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$17:$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>trend</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>tmin1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>tmin2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>tmin3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>tmin4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>tmin5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>tmin6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>tmin7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>tmin8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>tmin9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>tmin10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>tmin11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$17:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.27265949534124301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14591543663428175</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19416338748936296</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4401958437979899E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5585264293389438E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2899134158954736E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3762909203913068E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2993926771678873E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.9336451710931044E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.7975294803280271E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9171365540484892E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.1135375614500082E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6DF7-434A-9D35-23966EC2FE35}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="1693787792"/>
+        <c:axId val="1694283328"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1693787792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694283328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1694283328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1693787792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -14195,6 +14768,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -15242,6 +15855,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -15466,6 +16582,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86F311F1-2A0A-D14E-A3F6-D45EAA512EE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -30029,7 +31186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD05F54-52A0-5543-BE29-AD3A645F2976}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -30235,4 +31392,503 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A781923F-706A-364E-A816-F6B4334A1743}">
+  <dimension ref="A1:E28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1.5512485</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2.2012038</v>
+      </c>
+      <c r="D2" s="7">
+        <v>1.41898849</v>
+      </c>
+      <c r="E2" s="8">
+        <f>D2-100%</f>
+        <v>0.41898849000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6">
+        <v>8.4054696999999994</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1.177988</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0.14014541</v>
+      </c>
+      <c r="E3" s="8">
+        <f t="shared" ref="E3:E28" si="0">D3-100%</f>
+        <v>-0.85985458999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3.0188663999999998</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1.5674979</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.51923392000000002</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.48076607999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.78660330000000001</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.27772999999999998</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.35307507999999999</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.64692492000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.69235040000000003</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.3680138</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.53154265999999994</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.46845734000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.90527150000000001</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0.18486669999999999</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.20421136000000001</v>
+      </c>
+      <c r="E7" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.79578864000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2.0636543999999999</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0.2725709</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.13208168000000001</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.86791832000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1.1720967</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0.1049011</v>
+      </c>
+      <c r="D9" s="7">
+        <v>8.9498690000000006E-2</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.91050131000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="6">
+        <v>0.91153390000000001</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.55975920000000001</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.61408494999999996</v>
+      </c>
+      <c r="E10" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.38591505000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="6">
+        <v>2.5520412000000001</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.71023219999999998</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0.27829964000000001</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.72170036000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.75695599999999996</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.1547721</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.20446649</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.79553351000000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1.2854538</v>
+      </c>
+      <c r="C13" s="6">
+        <v>0.49355120000000002</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.38395090999999998</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="0"/>
+        <v>-0.61604908999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <f>SUM(B2:B13)</f>
+        <v>24.101545799999997</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C2:C13)</f>
+        <v>8.0730868999999998</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="5">
+        <f>B2/B$15</f>
+        <v>6.4363029362207974E-2</v>
+      </c>
+      <c r="C17" s="5">
+        <f>C2/C$15</f>
+        <v>0.27265949534124301</v>
+      </c>
+      <c r="D17" s="5">
+        <f>C17/B17</f>
+        <v>4.2362750486281557</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="5">
+        <f t="shared" ref="B18:C28" si="1">B3/B$15</f>
+        <v>0.34875230699932952</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14591543663428175</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ref="D18:D28" si="2">C18/B18</f>
+        <v>0.41839274954118733</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="5">
+        <f t="shared" si="1"/>
+        <v>0.12525613191167184</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="1"/>
+        <v>0.19416338748936296</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="2"/>
+        <v>1.5501307962015238</v>
+      </c>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
+        <f t="shared" si="1"/>
+        <v>3.2637047703388392E-2</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="1"/>
+        <v>3.4401958437979899E-2</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="2"/>
+        <v>1.0540769113257837</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5">
+        <f t="shared" si="1"/>
+        <v>2.8726389823510827E-2</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="1"/>
+        <v>4.5585264293389438E-2</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="2"/>
+        <v>1.5868775914222479</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5">
+        <f t="shared" si="1"/>
+        <v>3.7560723594749684E-2</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="1"/>
+        <v>2.2899134158954736E-2</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="2"/>
+        <v>0.60965636354661779</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5">
+        <f t="shared" si="1"/>
+        <v>8.5623321305806049E-2</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="1"/>
+        <v>3.3762909203913068E-2</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="2"/>
+        <v>0.39431907906641356</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" s="5">
+        <f t="shared" si="1"/>
+        <v>4.8631598559126452E-2</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="1"/>
+        <v>1.2993926771678873E-2</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2671910271647932</v>
+      </c>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="5">
+        <f t="shared" si="1"/>
+        <v>3.7820557551126038E-2</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="1"/>
+        <v>6.9336451710931044E-2</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="2"/>
+        <v>1.8333006227420536</v>
+      </c>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.10588703401754423</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="1"/>
+        <v>8.7975294803280271E-2</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="2"/>
+        <v>0.830841052632599</v>
+      </c>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" si="1"/>
+        <v>3.1406948180062379E-2</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="1"/>
+        <v>1.9171365540484892E-2</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="2"/>
+        <v>0.61041796963434913</v>
+      </c>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="5">
+        <f t="shared" si="1"/>
+        <v>5.3334910991476747E-2</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="1"/>
+        <v>6.1135375614500082E-2</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="2"/>
+        <v>1.1462543853175249</v>
+      </c>
+      <c r="E28" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>